<commit_message>
merged 5 Weighted MA  features  . 5 MA of diff  features , 5 historical average feature
</commit_message>
<xml_diff>
--- a/dataSource/testdata.xlsx
+++ b/dataSource/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A052C71B-6216-4592-986F-4231F76A2149}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D69D20-C76F-4C91-84E3-DD22AB4C0B3F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,10 +17,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -343,10 +339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D33" sqref="B19:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -572,6 +568,313 @@
         <v>0.827728423923631</v>
       </c>
     </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <v>8</v>
+      </c>
+      <c r="D35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>0.39872538696068099</v>
+      </c>
+      <c r="C36">
+        <v>0.63669992960508903</v>
+      </c>
+      <c r="D36">
+        <v>0.55338855268251896</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37">
+        <v>0.56789888052188198</v>
+      </c>
+      <c r="C37">
+        <v>0.68595166832307097</v>
+      </c>
+      <c r="D37">
+        <v>0.69857731869086603</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>3</v>
+      </c>
+      <c r="B38">
+        <v>0.58819291266663598</v>
+      </c>
+      <c r="C38">
+        <v>0.58554910996656695</v>
+      </c>
+      <c r="D38">
+        <v>0.64162764380307902</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="B39">
+        <v>0.97142857142857097</v>
+      </c>
+      <c r="C39">
+        <v>0.78333333333333299</v>
+      </c>
+      <c r="D39">
+        <v>0.78333333333333299</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>5</v>
+      </c>
+      <c r="B40">
+        <v>0.21709289840870499</v>
+      </c>
+      <c r="C40">
+        <v>0.77348633967487401</v>
+      </c>
+      <c r="D40">
+        <v>0.65643919332058098</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>6</v>
+      </c>
+      <c r="B41">
+        <v>0.80977260855035205</v>
+      </c>
+      <c r="C41">
+        <v>0.85890645140646305</v>
+      </c>
+      <c r="D41">
+        <v>0.87097017304880398</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>7</v>
+      </c>
+      <c r="B42">
+        <v>0.49157186808314002</v>
+      </c>
+      <c r="C42">
+        <v>0.77962180531827296</v>
+      </c>
+      <c r="D42">
+        <v>0.75003247650684501</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>8</v>
+      </c>
+      <c r="B43">
+        <v>0.63842240326949995</v>
+      </c>
+      <c r="C43">
+        <v>0.71380437246879802</v>
+      </c>
+      <c r="D43">
+        <v>0.71549199073222303</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>9</v>
+      </c>
+      <c r="B44">
+        <v>0.48012948391959198</v>
+      </c>
+      <c r="C44">
+        <v>0.37657079804439603</v>
+      </c>
+      <c r="D44">
+        <v>0.27083863185940699</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>10</v>
+      </c>
+      <c r="B45">
+        <v>0.53148189368865995</v>
+      </c>
+      <c r="C45">
+        <v>0.93058485984792305</v>
+      </c>
+      <c r="D45">
+        <v>0.91700779754205197</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>11</v>
+      </c>
+      <c r="B46">
+        <v>0.96803788186524997</v>
+      </c>
+      <c r="C46">
+        <v>0.96232866798739702</v>
+      </c>
+      <c r="D46">
+        <v>0.96648253525442696</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>12</v>
+      </c>
+      <c r="B47">
+        <v>0.35093217328895199</v>
+      </c>
+      <c r="C47">
+        <v>0.35682895678221199</v>
+      </c>
+      <c r="D47">
+        <v>0.34376888595194</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>13</v>
+      </c>
+      <c r="B48">
+        <v>0.69159378750413503</v>
+      </c>
+      <c r="C48">
+        <v>0.66284814929316105</v>
+      </c>
+      <c r="D48">
+        <v>0.68963495936008801</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>14</v>
+      </c>
+      <c r="B49">
+        <v>0.67215121233019404</v>
+      </c>
+      <c r="C49">
+        <v>0.73102141062633197</v>
+      </c>
+      <c r="D49">
+        <v>0.61726110688411695</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>15</v>
+      </c>
+      <c r="B50">
+        <v>0.61775702599888604</v>
+      </c>
+      <c r="C50">
+        <v>0.80111173615404996</v>
+      </c>
+      <c r="D50">
+        <v>0.82044578058469797</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>